<commit_message>
3-1-2025 Fixed spriteplot bug
</commit_message>
<xml_diff>
--- a/Suite system5/Doc/Sprite shift.xlsx
+++ b/Suite system5/Doc/Sprite shift.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="15">
   <si>
     <t>b0</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Sprite Shift Table:</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -365,6 +368,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -666,11 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AM269"/>
+  <dimension ref="B1:AS269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W22" sqref="W22"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK13" sqref="AK13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -694,11 +707,13 @@
     <col min="26" max="27" width="3.7109375" style="20" customWidth="1"/>
     <col min="28" max="29" width="3.7109375" style="5" customWidth="1"/>
     <col min="30" max="31" width="3.7109375" style="20" customWidth="1"/>
-    <col min="32" max="36" width="4.7109375" style="5" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="5"/>
+    <col min="32" max="35" width="4.7109375" style="5" customWidth="1"/>
+    <col min="36" max="36" width="4.7109375" style="34" customWidth="1"/>
+    <col min="37" max="37" width="3.7109375" style="34" customWidth="1"/>
+    <col min="38" max="44" width="3.7109375" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:45" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
         <v>13</v>
       </c>
@@ -714,12 +729,12 @@
       <c r="AG1" s="4"/>
       <c r="AH1" s="4"/>
       <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-    </row>
-    <row r="2" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+    </row>
+    <row r="2" spans="2:45" x14ac:dyDescent="0.25">
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -736,12 +751,12 @@
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-    </row>
-    <row r="4" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+    </row>
+    <row r="4" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -790,7 +805,7 @@
       <c r="W4" s="28"/>
       <c r="X4" s="32"/>
     </row>
-    <row r="5" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>32</v>
       </c>
@@ -901,8 +916,32 @@
       <c r="AF5" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="AK5" s="34">
+        <v>7</v>
+      </c>
+      <c r="AL5" s="35">
+        <v>6</v>
+      </c>
+      <c r="AM5" s="35">
+        <v>5</v>
+      </c>
+      <c r="AN5" s="35">
+        <v>4</v>
+      </c>
+      <c r="AO5" s="35">
+        <v>3</v>
+      </c>
+      <c r="AP5" s="35">
+        <v>2</v>
+      </c>
+      <c r="AQ5" s="35">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="11"/>
       <c r="D6" s="16"/>
@@ -954,8 +993,34 @@
       <c r="AF6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AJ6" s="38"/>
+      <c r="AK6" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL6" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN6" s="39">
+        <v>4</v>
+      </c>
+      <c r="AO6" s="39">
+        <v>3</v>
+      </c>
+      <c r="AP6" s="39">
+        <v>2</v>
+      </c>
+      <c r="AQ6" s="39">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="40"/>
+    </row>
+    <row r="7" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="11"/>
       <c r="D7" s="16"/>
@@ -1007,8 +1072,32 @@
       <c r="AF7" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK7" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL7" s="35">
+        <v>3</v>
+      </c>
+      <c r="AM7" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN7" s="35">
+        <v>2</v>
+      </c>
+      <c r="AO7" s="35">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="35">
+        <v>6</v>
+      </c>
+      <c r="AR7" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="27"/>
       <c r="C8" s="5"/>
       <c r="D8" s="34"/>
@@ -1034,8 +1123,32 @@
       <c r="X8" s="34"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
-    </row>
-    <row r="9" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="AK8" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL8" s="35">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN8" s="35">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="35">
+        <v>6</v>
+      </c>
+      <c r="AP8" s="35">
+        <v>4</v>
+      </c>
+      <c r="AQ8" s="35">
+        <v>3</v>
+      </c>
+      <c r="AR8" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>33</v>
       </c>
@@ -1147,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="11"/>
       <c r="D10" s="16"/>
@@ -1200,7 +1313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="11"/>
       <c r="D11" s="16"/>
@@ -1253,7 +1366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="34"/>
@@ -1281,7 +1394,7 @@
       <c r="AA12" s="5"/>
       <c r="AF12" s="4"/>
     </row>
-    <row r="13" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>34</v>
       </c>
@@ -1393,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="11"/>
       <c r="D14" s="16"/>
@@ -1446,7 +1559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="11"/>
       <c r="D15" s="16"/>
@@ -1499,7 +1612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="D16" s="34"/>

</xml_diff>